<commit_message>
Update xgb and build_library.
</commit_message>
<xml_diff>
--- a/build_Library/lipids_classification.xlsx
+++ b/build_Library/lipids_classification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fudan\Projects\2024\MultichannelR\Progress\build_package\MultichannelR\build_Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873A4CED-B1A8-4BE3-89C4-B3BCED8A11CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819EF88E-43A1-4059-B4B1-894E796597FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="300">
   <si>
     <t>class</t>
   </si>
@@ -1143,10 +1143,6 @@
   </si>
   <si>
     <t>detectable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>derivatizable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1154,7 +1150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1168,6 +1164,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1190,8 +1192,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1488,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,7 +1507,7 @@
     <col min="6" max="6" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1526,11 +1529,8 @@
       <c r="G1" t="s">
         <v>299</v>
       </c>
-      <c r="H1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1549,8 +1549,11 @@
       <c r="F2">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1569,8 +1572,11 @@
       <c r="F3">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1589,8 +1595,11 @@
       <c r="F4">
         <v>175</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1609,8 +1618,11 @@
       <c r="F5">
         <v>158</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1629,8 +1641,11 @@
       <c r="F6">
         <v>282</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1649,8 +1664,11 @@
       <c r="F7">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1669,8 +1687,11 @@
       <c r="F8">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1689,8 +1710,11 @@
       <c r="F9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1709,8 +1733,11 @@
       <c r="F10">
         <v>112</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1729,8 +1756,11 @@
       <c r="F11">
         <v>197</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1749,8 +1779,11 @@
       <c r="F12">
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1770,7 +1803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1790,7 +1823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1810,7 +1843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2154,7 +2187,7 @@
       <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">

</xml_diff>